<commit_message>
Sarath Track Of Sarath.xlsx updated
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -173,6 +173,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,7 +488,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,13 +1241,13 @@
       </c>
     </row>
     <row r="2" spans="1:247" ht="120" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1256,13 +1265,13 @@
       </c>
     </row>
     <row r="3" spans="1:247" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1272,13 +1281,13 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:247" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1298,13 +1307,13 @@
       </c>
     </row>
     <row r="5" spans="1:247" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">

</xml_diff>

<commit_message>
updated with Puzzle Try
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -182,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +491,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,10 +1287,10 @@
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">

</xml_diff>

<commit_message>
changes added..sry for not executing the programs... i will recover soon and ill get up to the mark...
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -499,8 +499,8 @@
   <dimension ref="A1:IM8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1284,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="6" t="s">
@@ -1302,7 +1302,7 @@
       <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1328,7 +1328,7 @@
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="5" t="s">

</xml_diff>

<commit_message>
Done some work after so much struggle.
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Things Done \ Date</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Merge Linked List at Alternate Position</t>
+  </si>
+  <si>
+    <t>Puzzle on soccer ball</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -234,6 +240,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,8 +551,8 @@
   <dimension ref="A1:IM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN15" sqref="AN15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +562,9 @@
     <col min="3" max="3" width="57" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="247" width="50.7109375" style="16" customWidth="1"/>
+    <col min="6" max="9" width="50.7109375" style="16" customWidth="1"/>
+    <col min="10" max="39" width="50.7109375" style="21" customWidth="1"/>
+    <col min="40" max="247" width="50.7109375" style="16" customWidth="1"/>
     <col min="248" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
@@ -582,94 +596,94 @@
       <c r="I1" s="1">
         <v>41565</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="20">
         <v>41566</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="20">
         <v>41567</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="20">
         <v>41568</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="20">
         <v>41569</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="20">
         <v>41570</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="20">
         <v>41571</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="20">
         <v>41572</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="20">
         <v>41573</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="20">
         <v>41574</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1" s="20">
         <v>41575</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1" s="20">
         <v>41576</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1" s="20">
         <v>41577</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V1" s="20">
         <v>41578</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W1" s="20">
         <v>41579</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X1" s="20">
         <v>41580</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y1" s="20">
         <v>41581</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z1" s="20">
         <v>41582</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA1" s="20">
         <v>41583</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB1" s="20">
         <v>41584</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC1" s="20">
         <v>41585</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD1" s="20">
         <v>41586</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE1" s="20">
         <v>41587</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF1" s="20">
         <v>41588</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AG1" s="20">
         <v>41589</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AH1" s="20">
         <v>41590</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AI1" s="20">
         <v>41591</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AJ1" s="20">
         <v>41592</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AK1" s="20">
         <v>41593</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AL1" s="20">
         <v>41594</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AM1" s="20">
         <v>41595</v>
       </c>
       <c r="AN1" s="1">
@@ -1323,37 +1337,39 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5"/>
       <c r="AQ2" s="5"/>
@@ -1580,37 +1596,39 @@
         <v>18</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
       <c r="AQ3" s="5"/>
@@ -1847,37 +1865,37 @@
       <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="5"/>
-      <c r="AN4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="4"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="5"/>
       <c r="AQ4" s="5"/>
@@ -2111,37 +2129,37 @@
       <c r="I5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="17"/>
       <c r="AO5" s="14"/>
       <c r="AP5" s="14"/>
       <c r="AQ5" s="14"/>

</xml_diff>

<commit_message>
sothapping...but not giving up..im tryin....
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="20700" windowHeight="9975"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="20610" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Things Done \ Date</t>
   </si>
@@ -153,12 +153,40 @@
     <t>Given an array and two numbers x and y, 
 find minimum distance between two numbers x and y. assume that x and y always exist in array and it may be that x and y are same also…</t>
   </si>
+  <si>
+    <t>3.Given a linked list and 2 integers M and N.Keep M nodes and delete N nodes repetitively till the end of linkedlist.</t>
+  </si>
+  <si>
+    <r>
+      <t>2.Find Nth largest element in the BST.(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trying it but sothapping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +204,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -619,7 +654,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BB3" sqref="BB3"/>
+      <selection pane="topRight" activeCell="BB10" sqref="BB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1458,8 +1493,8 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
       <c r="BA2" s="3"/>
-      <c r="BB2" s="7" t="s">
-        <v>28</v>
+      <c r="BB2" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="BC2" s="23" t="s">
         <v>16</v>
@@ -1734,7 +1769,7 @@
       <c r="AZ3" s="3"/>
       <c r="BA3" s="3"/>
       <c r="BB3" s="25" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="BC3" s="24" t="s">
         <v>37</v>
@@ -2006,7 +2041,7 @@
       <c r="AY4" s="5"/>
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
-      <c r="BB4" s="23" t="s">
+      <c r="BB4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="BC4" s="23" t="s">

</xml_diff>

<commit_message>
updated videos with red. Positive Thoughts gained cuz of agent p ... Thank You agent P for teaching important lesson in my life :) ...
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Things Done \ Date</t>
   </si>
@@ -179,21 +179,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Given a BST , replace a node value with the sum of all the elements larger than the current node.-Execute </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>( But Having Trouble Assigning Value , Logic is correct , Error at pointer arithmetic)</t>
     </r>
   </si>
 </sst>
@@ -672,7 +657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BD3" sqref="BD3"/>
+      <selection pane="topRight" activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1515,7 +1500,7 @@
         <v>43</v>
       </c>
       <c r="BC2" s="19" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="BD2" s="19" t="s">
         <v>39</v>
@@ -2062,16 +2047,16 @@
       <c r="BB4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="BC4" s="23" t="s">
+      <c r="BC4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="BD4" s="23" t="s">
+      <c r="BD4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BE4" s="23" t="s">
+      <c r="BE4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BF4" s="23" t="s">
+      <c r="BF4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="BG4" s="23" t="s">

</xml_diff>

<commit_message>
Updated without doing anything...sorry ....:(
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -285,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -343,9 +343,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -659,8 +656,8 @@
   <dimension ref="A1:IM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BK13" sqref="BK13"/>
+      <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1498,7 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
       <c r="BA2" s="3"/>
-      <c r="BB2" s="26" t="s">
+      <c r="BB2" s="25" t="s">
         <v>47</v>
       </c>
       <c r="BC2" s="19" t="s">
@@ -1524,13 +1521,13 @@
       <c r="BJ2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="BK2" s="27" t="s">
+      <c r="BK2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="BL2" s="25" t="s">
+      <c r="BL2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="BM2" s="25" t="s">
+      <c r="BM2" s="26" t="s">
         <v>45</v>
       </c>
       <c r="BN2" s="5"/>
@@ -1806,8 +1803,8 @@
         <v>46</v>
       </c>
       <c r="BK3" s="3"/>
-      <c r="BL3" s="23"/>
-      <c r="BM3" s="23"/>
+      <c r="BL3" s="3"/>
+      <c r="BM3" s="3"/>
       <c r="BN3" s="5"/>
       <c r="BO3" s="5"/>
       <c r="BP3" s="5"/>
@@ -2091,10 +2088,10 @@
       <c r="BK4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BL4" s="23" t="s">
+      <c r="BL4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BM4" s="23" t="s">
+      <c r="BM4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="BN4" s="5"/>

</xml_diff>

<commit_message>
Track Of Sarath.xlsx updated..
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -656,8 +656,8 @@
   <dimension ref="A1:IM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CF8" sqref="CF8"/>
+      <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CI10" sqref="CI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,10 +1549,10 @@
       <c r="CD2" s="3"/>
       <c r="CE2" s="3"/>
       <c r="CF2" s="3"/>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-      <c r="CJ2" s="5"/>
+      <c r="CG2" s="3"/>
+      <c r="CH2" s="3"/>
+      <c r="CI2" s="3"/>
+      <c r="CJ2" s="3"/>
       <c r="CK2" s="5"/>
       <c r="CL2" s="5"/>
       <c r="CM2" s="5"/>
@@ -1824,10 +1824,10 @@
       <c r="CD3" s="3"/>
       <c r="CE3" s="3"/>
       <c r="CF3" s="3"/>
-      <c r="CG3" s="5"/>
-      <c r="CH3" s="5"/>
-      <c r="CI3" s="5"/>
-      <c r="CJ3" s="5"/>
+      <c r="CG3" s="3"/>
+      <c r="CH3" s="3"/>
+      <c r="CI3" s="3"/>
+      <c r="CJ3" s="3"/>
       <c r="CK3" s="5"/>
       <c r="CL3" s="5"/>
       <c r="CM3" s="5"/>
@@ -2113,10 +2113,10 @@
       <c r="CD4" s="3"/>
       <c r="CE4" s="3"/>
       <c r="CF4" s="3"/>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-      <c r="CJ4" s="5"/>
+      <c r="CG4" s="3"/>
+      <c r="CH4" s="3"/>
+      <c r="CI4" s="3"/>
+      <c r="CJ4" s="3"/>
       <c r="CK4" s="5"/>
       <c r="CL4" s="5"/>
       <c r="CM4" s="5"/>
@@ -2377,10 +2377,10 @@
       <c r="CD5" s="18"/>
       <c r="CE5" s="18"/>
       <c r="CF5" s="18"/>
-      <c r="CG5" s="14"/>
-      <c r="CH5" s="14"/>
-      <c r="CI5" s="14"/>
-      <c r="CJ5" s="14"/>
+      <c r="CG5" s="18"/>
+      <c r="CH5" s="18"/>
+      <c r="CI5" s="18"/>
+      <c r="CJ5" s="18"/>
       <c r="CK5" s="14"/>
       <c r="CL5" s="14"/>
       <c r="CM5" s="14"/>

</xml_diff>

<commit_message>
Updated Track Of Sarath.xlsx
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -729,8 +729,8 @@
   <dimension ref="A1:IM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EI6" sqref="EI6"/>
+      <pane xSplit="1" topLeftCell="EP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EH10" sqref="EH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,16 +1688,16 @@
       <c r="EF2" s="2"/>
       <c r="EG2" s="2"/>
       <c r="EH2" s="2"/>
-      <c r="EI2" s="4"/>
-      <c r="EJ2" s="4"/>
-      <c r="EK2" s="4"/>
-      <c r="EL2" s="4"/>
-      <c r="EM2" s="4"/>
-      <c r="EN2" s="4"/>
-      <c r="EO2" s="4"/>
-      <c r="EP2" s="4"/>
-      <c r="EQ2" s="4"/>
-      <c r="ER2" s="4"/>
+      <c r="EI2" s="2"/>
+      <c r="EJ2" s="2"/>
+      <c r="EK2" s="2"/>
+      <c r="EL2" s="2"/>
+      <c r="EM2" s="2"/>
+      <c r="EN2" s="2"/>
+      <c r="EO2" s="2"/>
+      <c r="EP2" s="2"/>
+      <c r="EQ2" s="2"/>
+      <c r="ER2" s="2"/>
       <c r="ES2" s="4"/>
       <c r="ET2" s="4"/>
       <c r="EU2" s="4"/>
@@ -1973,16 +1973,16 @@
       <c r="EF3" s="2"/>
       <c r="EG3" s="2"/>
       <c r="EH3" s="2"/>
-      <c r="EI3" s="4"/>
-      <c r="EJ3" s="4"/>
-      <c r="EK3" s="4"/>
-      <c r="EL3" s="4"/>
-      <c r="EM3" s="4"/>
-      <c r="EN3" s="4"/>
-      <c r="EO3" s="4"/>
-      <c r="EP3" s="4"/>
-      <c r="EQ3" s="4"/>
-      <c r="ER3" s="4"/>
+      <c r="EI3" s="2"/>
+      <c r="EJ3" s="2"/>
+      <c r="EK3" s="2"/>
+      <c r="EL3" s="2"/>
+      <c r="EM3" s="2"/>
+      <c r="EN3" s="2"/>
+      <c r="EO3" s="2"/>
+      <c r="EP3" s="2"/>
+      <c r="EQ3" s="2"/>
+      <c r="ER3" s="2"/>
       <c r="ES3" s="4"/>
       <c r="ET3" s="4"/>
       <c r="EU3" s="4"/>
@@ -2268,16 +2268,16 @@
       <c r="EF4" s="2"/>
       <c r="EG4" s="2"/>
       <c r="EH4" s="2"/>
-      <c r="EI4" s="4"/>
-      <c r="EJ4" s="4"/>
-      <c r="EK4" s="4"/>
-      <c r="EL4" s="4"/>
-      <c r="EM4" s="4"/>
-      <c r="EN4" s="4"/>
-      <c r="EO4" s="4"/>
-      <c r="EP4" s="4"/>
-      <c r="EQ4" s="4"/>
-      <c r="ER4" s="4"/>
+      <c r="EI4" s="2"/>
+      <c r="EJ4" s="2"/>
+      <c r="EK4" s="2"/>
+      <c r="EL4" s="2"/>
+      <c r="EM4" s="2"/>
+      <c r="EN4" s="2"/>
+      <c r="EO4" s="2"/>
+      <c r="EP4" s="2"/>
+      <c r="EQ4" s="2"/>
+      <c r="ER4" s="2"/>
       <c r="ES4" s="4"/>
       <c r="ET4" s="4"/>
       <c r="EU4" s="4"/>
@@ -2534,16 +2534,16 @@
       <c r="EF5" s="17"/>
       <c r="EG5" s="17"/>
       <c r="EH5" s="17"/>
-      <c r="EI5" s="13"/>
-      <c r="EJ5" s="13"/>
-      <c r="EK5" s="13"/>
-      <c r="EL5" s="13"/>
-      <c r="EM5" s="13"/>
-      <c r="EN5" s="13"/>
-      <c r="EO5" s="13"/>
-      <c r="EP5" s="13"/>
-      <c r="EQ5" s="13"/>
-      <c r="ER5" s="13"/>
+      <c r="EI5" s="17"/>
+      <c r="EJ5" s="17"/>
+      <c r="EK5" s="17"/>
+      <c r="EL5" s="17"/>
+      <c r="EM5" s="17"/>
+      <c r="EN5" s="17"/>
+      <c r="EO5" s="17"/>
+      <c r="EP5" s="17"/>
+      <c r="EQ5" s="17"/>
+      <c r="ER5" s="17"/>
       <c r="ES5" s="13"/>
       <c r="ET5" s="13"/>
       <c r="EU5" s="13"/>

</xml_diff>

<commit_message>
Ideas Added Track Of Sarath.xlsx updated.
</commit_message>
<xml_diff>
--- a/Track Of Sarath.xlsx
+++ b/Track Of Sarath.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
   <si>
     <t>Things Done \ Date</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>2) Sherlock and The Beast</t>
+  </si>
+  <si>
+    <t>1)AngryChildren</t>
+  </si>
+  <si>
+    <t>2)Sherlock and the Beast</t>
+  </si>
+  <si>
+    <t>3)Maximizing Xor</t>
   </si>
 </sst>
 </file>
@@ -775,8 +784,8 @@
   <dimension ref="A1:IM5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="GG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="GI5" sqref="GI5"/>
+      <pane xSplit="1" topLeftCell="GJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GK9" sqref="GK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1804,9 @@
       </c>
       <c r="GJ2" s="31"/>
       <c r="GK2" s="31"/>
-      <c r="GL2" s="4"/>
+      <c r="GL2" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="GM2" s="4"/>
       <c r="GN2" s="4"/>
       <c r="GO2" s="4"/>
@@ -2086,7 +2097,9 @@
       </c>
       <c r="GJ3" s="31"/>
       <c r="GK3" s="31"/>
-      <c r="GL3" s="4"/>
+      <c r="GL3" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="GM3" s="4"/>
       <c r="GN3" s="4"/>
       <c r="GO3" s="4"/>
@@ -2383,7 +2396,9 @@
       <c r="GI4" s="31"/>
       <c r="GJ4" s="31"/>
       <c r="GK4" s="31"/>
-      <c r="GL4" s="4"/>
+      <c r="GL4" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="GM4" s="4"/>
       <c r="GN4" s="4"/>
       <c r="GO4" s="4"/>
@@ -2651,7 +2666,7 @@
       <c r="GI5" s="32"/>
       <c r="GJ5" s="32"/>
       <c r="GK5" s="32"/>
-      <c r="GL5" s="13"/>
+      <c r="GL5" s="17"/>
       <c r="GM5" s="13"/>
       <c r="GN5" s="13"/>
       <c r="GO5" s="13"/>

</xml_diff>